<commit_message>
Spiegazione a Cavallina e Sandro
</commit_message>
<xml_diff>
--- a/Config/Config_test.xlsx
+++ b/Config/Config_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITLOAIT\Documents\GitHub\OrionLogger\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42803FAE-87C4-4F19-AA97-51257846C618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1EE223-1700-4E4E-9DD2-FF8721B94B53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>STRUMENTI</t>
-  </si>
-  <si>
     <t>CICLO</t>
   </si>
   <si>
@@ -52,12 +49,6 @@
     <t>COLONNINA_PORTA</t>
   </si>
   <si>
-    <t>sss</t>
-  </si>
-  <si>
-    <t>Alimentatore</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -70,21 +61,12 @@
     <t>COM3</t>
   </si>
   <si>
-    <t>Arduino</t>
-  </si>
-  <si>
     <t>GPIB0::28::INSTR</t>
   </si>
   <si>
-    <t>Camera Climatica</t>
-  </si>
-  <si>
     <t>TEMPO</t>
   </si>
   <si>
-    <t>EVENTO</t>
-  </si>
-  <si>
     <t>CC_ON/OFF</t>
   </si>
   <si>
@@ -143,13 +125,31 @@
   </si>
   <si>
     <t>COL_VAL</t>
+  </si>
+  <si>
+    <t>ALIM_CURVAID</t>
+  </si>
+  <si>
+    <t>ALIMENTATORE _CURVA</t>
+  </si>
+  <si>
+    <t>ALIMENTATORE _CURVAID</t>
+  </si>
+  <si>
+    <t>CC_ID</t>
+  </si>
+  <si>
+    <t>Weiss</t>
+  </si>
+  <si>
+    <t>Automatico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -166,13 +166,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -234,19 +227,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -327,11 +307,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -341,9 +332,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -363,15 +351,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -875,82 +861,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ4"/>
+  <dimension ref="A1:AML3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" style="1" customWidth="1"/>
-    <col min="9" max="1024" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="21.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.44140625" style="1" customWidth="1"/>
+    <col min="11" max="1026" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -961,24 +951,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13.33203125" customWidth="1"/>
     <col min="13" max="14" width="13.33203125" hidden="1" customWidth="1"/>
     <col min="15" max="16" width="13.33203125" customWidth="1"/>
@@ -986,126 +976,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="J1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="L1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="M1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="N1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="O1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="P1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="S1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="T1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="U1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="V1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A2" s="12">
+      <c r="A2" s="10">
         <v>15</v>
       </c>
-      <c r="B2" s="12">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12">
-        <v>2</v>
-      </c>
-      <c r="D2" s="12">
-        <v>0</v>
-      </c>
-      <c r="E2" s="12">
-        <v>0</v>
-      </c>
-      <c r="F2" s="13">
-        <v>2</v>
-      </c>
-      <c r="G2" s="12">
+      <c r="B2" s="10">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
+        <v>2</v>
+      </c>
+      <c r="F2" s="10">
         <v>610</v>
       </c>
-      <c r="H2" s="12">
-        <v>1</v>
-      </c>
-      <c r="I2" s="12">
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10">
         <v>100</v>
       </c>
-      <c r="J2" s="12">
-        <v>0</v>
-      </c>
-      <c r="K2" s="12">
-        <v>2</v>
-      </c>
-      <c r="L2" s="12">
-        <v>0</v>
-      </c>
-      <c r="M2" s="12">
-        <v>2</v>
-      </c>
-      <c r="N2" s="12">
-        <v>2</v>
-      </c>
-      <c r="O2" s="12">
-        <v>2</v>
-      </c>
-      <c r="P2" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="12">
-        <v>2</v>
-      </c>
-      <c r="R2" s="12">
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2" s="11">
+        <v>0</v>
+      </c>
+      <c r="K2" s="10">
+        <v>2</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0</v>
+      </c>
+      <c r="M2" s="10">
+        <v>2</v>
+      </c>
+      <c r="N2" s="10">
+        <v>2</v>
+      </c>
+      <c r="O2" s="10">
+        <v>2</v>
+      </c>
+      <c r="P2" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>2</v>
+      </c>
+      <c r="R2" s="10">
         <v>2</v>
       </c>
       <c r="S2">
@@ -1122,58 +1112,58 @@
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+      <c r="A3" s="10">
         <v>10</v>
       </c>
-      <c r="B3" s="12">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12">
-        <v>2</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" s="13">
-        <v>2</v>
-      </c>
-      <c r="G3" s="12">
+      <c r="B3" s="10">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11">
+        <v>2</v>
+      </c>
+      <c r="F3" s="10">
         <v>610</v>
       </c>
-      <c r="H3" s="12">
-        <v>1</v>
-      </c>
-      <c r="I3" s="12">
+      <c r="G3" s="10">
+        <v>1</v>
+      </c>
+      <c r="H3" s="10">
         <v>100</v>
       </c>
-      <c r="J3" s="12">
-        <v>0</v>
-      </c>
-      <c r="K3" s="12">
-        <v>0</v>
-      </c>
-      <c r="L3" s="12">
-        <v>2</v>
-      </c>
-      <c r="M3" s="12">
-        <v>2</v>
-      </c>
-      <c r="N3" s="12">
-        <v>2</v>
-      </c>
-      <c r="O3" s="12">
-        <v>0</v>
-      </c>
-      <c r="P3" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="12">
-        <v>2</v>
-      </c>
-      <c r="R3" s="12">
+      <c r="I3" s="10">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11">
+        <v>0</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0</v>
+      </c>
+      <c r="L3" s="10">
+        <v>2</v>
+      </c>
+      <c r="M3" s="10">
+        <v>2</v>
+      </c>
+      <c r="N3" s="10">
+        <v>2</v>
+      </c>
+      <c r="O3" s="10">
+        <v>0</v>
+      </c>
+      <c r="P3" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>2</v>
+      </c>
+      <c r="R3" s="10">
         <v>2</v>
       </c>
       <c r="S3">
@@ -1190,58 +1180,58 @@
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="10">
         <v>10</v>
       </c>
-      <c r="B4" s="12">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12">
-        <v>2</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12">
-        <v>0</v>
-      </c>
-      <c r="F4" s="13">
-        <v>2</v>
-      </c>
-      <c r="G4" s="12">
+      <c r="B4" s="10">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2</v>
+      </c>
+      <c r="F4" s="10">
         <v>610</v>
       </c>
-      <c r="H4" s="12">
-        <v>1</v>
-      </c>
-      <c r="I4" s="12">
+      <c r="G4" s="10">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10">
         <v>100</v>
       </c>
-      <c r="J4" s="12">
-        <v>0</v>
-      </c>
-      <c r="K4" s="12">
-        <v>2</v>
-      </c>
-      <c r="L4" s="12">
-        <v>2</v>
-      </c>
-      <c r="M4" s="12">
-        <v>2</v>
-      </c>
-      <c r="N4" s="12">
-        <v>2</v>
-      </c>
-      <c r="O4" s="12">
-        <v>1</v>
-      </c>
-      <c r="P4" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="12">
-        <v>2</v>
-      </c>
-      <c r="R4" s="12">
+      <c r="I4" s="10">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
+        <v>0</v>
+      </c>
+      <c r="K4" s="10">
+        <v>2</v>
+      </c>
+      <c r="L4" s="10">
+        <v>2</v>
+      </c>
+      <c r="M4" s="10">
+        <v>2</v>
+      </c>
+      <c r="N4" s="10">
+        <v>2</v>
+      </c>
+      <c r="O4" s="10">
+        <v>1</v>
+      </c>
+      <c r="P4" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>2</v>
+      </c>
+      <c r="R4" s="10">
         <v>2</v>
       </c>
       <c r="S4">
@@ -1258,58 +1248,58 @@
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+      <c r="A5" s="10">
         <v>10</v>
       </c>
-      <c r="B5" s="12">
-        <v>0</v>
-      </c>
-      <c r="C5" s="12">
-        <v>2</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0</v>
-      </c>
-      <c r="E5" s="12">
-        <v>0</v>
-      </c>
-      <c r="F5" s="13">
-        <v>2</v>
-      </c>
-      <c r="G5" s="12">
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10">
         <v>610</v>
       </c>
-      <c r="H5" s="12">
-        <v>1</v>
-      </c>
-      <c r="I5" s="12">
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10">
         <v>100</v>
       </c>
-      <c r="J5" s="12">
-        <v>0</v>
-      </c>
-      <c r="K5" s="12">
-        <v>1</v>
-      </c>
-      <c r="L5" s="12">
-        <v>2</v>
-      </c>
-      <c r="M5" s="12">
-        <v>2</v>
-      </c>
-      <c r="N5" s="12">
-        <v>2</v>
-      </c>
-      <c r="O5" s="12">
-        <v>2</v>
-      </c>
-      <c r="P5" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="12">
-        <v>2</v>
-      </c>
-      <c r="R5" s="12">
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
+        <v>0</v>
+      </c>
+      <c r="K5" s="10">
+        <v>1</v>
+      </c>
+      <c r="L5" s="10">
+        <v>2</v>
+      </c>
+      <c r="M5" s="10">
+        <v>2</v>
+      </c>
+      <c r="N5" s="10">
+        <v>2</v>
+      </c>
+      <c r="O5" s="10">
+        <v>2</v>
+      </c>
+      <c r="P5" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="10">
+        <v>2</v>
+      </c>
+      <c r="R5" s="10">
         <v>2</v>
       </c>
       <c r="S5">
@@ -1326,58 +1316,58 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+      <c r="A6" s="12">
         <v>10</v>
       </c>
-      <c r="B6" s="14">
-        <v>0</v>
-      </c>
-      <c r="C6" s="12">
-        <v>2</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0</v>
-      </c>
-      <c r="E6" s="12">
-        <v>0</v>
-      </c>
-      <c r="F6" s="15">
-        <v>2</v>
-      </c>
-      <c r="G6" s="12">
+      <c r="B6" s="10">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10">
         <v>610</v>
       </c>
-      <c r="H6" s="12">
-        <v>1</v>
-      </c>
-      <c r="I6" s="12">
+      <c r="G6" s="10">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10">
         <v>100</v>
       </c>
-      <c r="J6" s="12">
-        <v>0</v>
-      </c>
-      <c r="K6" s="12">
-        <v>2</v>
-      </c>
-      <c r="L6" s="12">
-        <v>2</v>
-      </c>
-      <c r="M6" s="16">
-        <v>2</v>
-      </c>
-      <c r="N6" s="16">
-        <v>2</v>
-      </c>
-      <c r="O6" s="16">
-        <v>2</v>
-      </c>
-      <c r="P6" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="16">
-        <v>2</v>
-      </c>
-      <c r="R6" s="12">
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
+        <v>0</v>
+      </c>
+      <c r="K6" s="10">
+        <v>2</v>
+      </c>
+      <c r="L6" s="10">
+        <v>2</v>
+      </c>
+      <c r="M6" s="14">
+        <v>2</v>
+      </c>
+      <c r="N6" s="14">
+        <v>2</v>
+      </c>
+      <c r="O6" s="14">
+        <v>2</v>
+      </c>
+      <c r="P6" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>2</v>
+      </c>
+      <c r="R6" s="10">
         <v>2</v>
       </c>
       <c r="S6">
@@ -1394,58 +1384,58 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="14">
         <v>30</v>
       </c>
-      <c r="B7" s="16">
-        <v>0</v>
-      </c>
-      <c r="C7" s="12">
-        <v>2</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12">
-        <v>0</v>
-      </c>
-      <c r="F7" s="17">
-        <v>2</v>
-      </c>
-      <c r="G7" s="12">
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="15">
+        <v>2</v>
+      </c>
+      <c r="F7" s="10">
         <v>610</v>
       </c>
-      <c r="H7" s="12">
-        <v>1</v>
-      </c>
-      <c r="I7" s="12">
+      <c r="G7" s="10">
+        <v>1</v>
+      </c>
+      <c r="H7" s="10">
         <v>100</v>
       </c>
-      <c r="J7" s="12">
-        <v>0</v>
-      </c>
-      <c r="K7" s="12">
-        <v>2</v>
-      </c>
-      <c r="L7" s="12">
-        <v>1</v>
-      </c>
-      <c r="M7" s="16">
-        <v>2</v>
-      </c>
-      <c r="N7" s="16">
-        <v>2</v>
-      </c>
-      <c r="O7" s="16">
-        <v>2</v>
-      </c>
-      <c r="P7" s="16">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="16">
-        <v>2</v>
-      </c>
-      <c r="R7" s="12">
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0</v>
+      </c>
+      <c r="K7" s="10">
+        <v>2</v>
+      </c>
+      <c r="L7" s="10">
+        <v>1</v>
+      </c>
+      <c r="M7" s="14">
+        <v>2</v>
+      </c>
+      <c r="N7" s="14">
+        <v>2</v>
+      </c>
+      <c r="O7" s="14">
+        <v>2</v>
+      </c>
+      <c r="P7" s="14">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>2</v>
+      </c>
+      <c r="R7" s="10">
         <v>2</v>
       </c>
       <c r="S7">
@@ -1462,58 +1452,58 @@
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
+      <c r="A8" s="14">
         <v>75</v>
       </c>
-      <c r="B8" s="16">
-        <v>0</v>
-      </c>
-      <c r="C8" s="12">
-        <v>2</v>
-      </c>
-      <c r="D8" s="12">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12">
-        <v>0</v>
-      </c>
-      <c r="F8" s="17">
-        <v>1</v>
-      </c>
-      <c r="G8" s="12">
+      <c r="B8" s="10">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="15">
+        <v>1</v>
+      </c>
+      <c r="F8" s="10">
         <v>610</v>
       </c>
-      <c r="H8" s="12">
+      <c r="G8" s="10">
         <v>15</v>
       </c>
-      <c r="I8" s="12">
+      <c r="H8" s="10">
         <v>20000</v>
       </c>
-      <c r="J8" s="12">
-        <v>0</v>
-      </c>
-      <c r="K8" s="12">
-        <v>2</v>
-      </c>
-      <c r="L8" s="12">
-        <v>2</v>
-      </c>
-      <c r="M8" s="12">
-        <v>2</v>
-      </c>
-      <c r="N8" s="12">
-        <v>2</v>
-      </c>
-      <c r="O8" s="12">
-        <v>2</v>
-      </c>
-      <c r="P8" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="12">
-        <v>2</v>
-      </c>
-      <c r="R8" s="12">
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <v>2</v>
+      </c>
+      <c r="L8" s="10">
+        <v>2</v>
+      </c>
+      <c r="M8" s="10">
+        <v>2</v>
+      </c>
+      <c r="N8" s="10">
+        <v>2</v>
+      </c>
+      <c r="O8" s="10">
+        <v>2</v>
+      </c>
+      <c r="P8" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>2</v>
+      </c>
+      <c r="R8" s="10">
         <v>2</v>
       </c>
       <c r="S8">
@@ -1530,58 +1520,58 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
+      <c r="A9" s="14">
         <v>15</v>
       </c>
-      <c r="B9" s="16">
-        <v>0</v>
-      </c>
-      <c r="C9" s="12">
-        <v>2</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0</v>
-      </c>
-      <c r="E9" s="12">
-        <v>0</v>
-      </c>
-      <c r="F9" s="17">
-        <v>1</v>
-      </c>
-      <c r="G9" s="12">
+      <c r="B9" s="10">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
         <v>610</v>
       </c>
-      <c r="H9" s="12">
+      <c r="G9" s="10">
         <v>28</v>
       </c>
-      <c r="I9" s="12">
+      <c r="H9" s="10">
         <v>20000</v>
       </c>
-      <c r="J9" s="12">
-        <v>0</v>
-      </c>
-      <c r="K9" s="12">
-        <v>2</v>
-      </c>
-      <c r="L9" s="12">
-        <v>2</v>
-      </c>
-      <c r="M9" s="12">
-        <v>2</v>
-      </c>
-      <c r="N9" s="12">
-        <v>2</v>
-      </c>
-      <c r="O9" s="12">
-        <v>2</v>
-      </c>
-      <c r="P9" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="12">
-        <v>2</v>
-      </c>
-      <c r="R9" s="12">
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <v>2</v>
+      </c>
+      <c r="L9" s="10">
+        <v>2</v>
+      </c>
+      <c r="M9" s="10">
+        <v>2</v>
+      </c>
+      <c r="N9" s="10">
+        <v>2</v>
+      </c>
+      <c r="O9" s="10">
+        <v>2</v>
+      </c>
+      <c r="P9" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>2</v>
+      </c>
+      <c r="R9" s="10">
         <v>2</v>
       </c>
       <c r="S9">
@@ -1598,58 +1588,58 @@
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
+      <c r="A10" s="14">
         <v>60</v>
       </c>
-      <c r="B10" s="16">
-        <v>0</v>
-      </c>
-      <c r="C10" s="12">
-        <v>2</v>
-      </c>
-      <c r="D10" s="12">
-        <v>0</v>
-      </c>
-      <c r="E10" s="12">
-        <v>0</v>
-      </c>
-      <c r="F10" s="17">
-        <v>1</v>
-      </c>
-      <c r="G10" s="12">
+      <c r="B10" s="10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
         <v>610</v>
       </c>
-      <c r="H10" s="12">
+      <c r="G10" s="10">
         <v>35</v>
       </c>
-      <c r="I10" s="12">
+      <c r="H10" s="10">
         <v>20000</v>
       </c>
-      <c r="J10" s="12">
-        <v>0</v>
-      </c>
-      <c r="K10" s="12">
-        <v>2</v>
-      </c>
-      <c r="L10" s="12">
-        <v>2</v>
-      </c>
-      <c r="M10" s="12">
-        <v>2</v>
-      </c>
-      <c r="N10" s="12">
-        <v>2</v>
-      </c>
-      <c r="O10" s="12">
-        <v>2</v>
-      </c>
-      <c r="P10" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="12">
-        <v>2</v>
-      </c>
-      <c r="R10" s="12">
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="11">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10">
+        <v>2</v>
+      </c>
+      <c r="L10" s="10">
+        <v>2</v>
+      </c>
+      <c r="M10" s="10">
+        <v>2</v>
+      </c>
+      <c r="N10" s="10">
+        <v>2</v>
+      </c>
+      <c r="O10" s="10">
+        <v>2</v>
+      </c>
+      <c r="P10" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>2</v>
+      </c>
+      <c r="R10" s="10">
         <v>2</v>
       </c>
       <c r="S10">
@@ -1666,58 +1656,58 @@
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="10">
         <v>5</v>
       </c>
-      <c r="B11" s="12">
-        <v>0</v>
-      </c>
-      <c r="C11" s="12">
-        <v>2</v>
-      </c>
-      <c r="D11" s="12">
-        <v>0</v>
-      </c>
-      <c r="E11" s="12">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13">
-        <v>1</v>
-      </c>
-      <c r="G11" s="12">
+      <c r="B11" s="10">
+        <v>2</v>
+      </c>
+      <c r="C11" s="10">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="10">
         <v>610</v>
       </c>
-      <c r="H11" s="12">
-        <v>1</v>
-      </c>
-      <c r="I11" s="12">
+      <c r="G11" s="10">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10">
         <v>100</v>
       </c>
-      <c r="J11" s="12">
-        <v>0</v>
-      </c>
-      <c r="K11" s="12">
-        <v>2</v>
-      </c>
-      <c r="L11" s="12">
-        <v>2</v>
-      </c>
-      <c r="M11" s="12">
-        <v>2</v>
-      </c>
-      <c r="N11" s="12">
-        <v>2</v>
-      </c>
-      <c r="O11" s="12">
-        <v>2</v>
-      </c>
-      <c r="P11" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="12">
-        <v>2</v>
-      </c>
-      <c r="R11" s="12">
+      <c r="I11" s="10">
+        <v>0</v>
+      </c>
+      <c r="J11" s="11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="10">
+        <v>2</v>
+      </c>
+      <c r="L11" s="10">
+        <v>2</v>
+      </c>
+      <c r="M11" s="10">
+        <v>2</v>
+      </c>
+      <c r="N11" s="10">
+        <v>2</v>
+      </c>
+      <c r="O11" s="10">
+        <v>2</v>
+      </c>
+      <c r="P11" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>2</v>
+      </c>
+      <c r="R11" s="10">
         <v>2</v>
       </c>
       <c r="S11">
@@ -1734,58 +1724,58 @@
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="A12" s="10">
         <v>5</v>
       </c>
-      <c r="B12" s="12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0</v>
-      </c>
-      <c r="E12" s="12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="13">
-        <v>2</v>
-      </c>
-      <c r="G12" s="12">
+      <c r="B12" s="10">
+        <v>2</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0</v>
+      </c>
+      <c r="E12" s="11">
+        <v>2</v>
+      </c>
+      <c r="F12" s="10">
         <v>610</v>
       </c>
-      <c r="H12" s="12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="12">
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10">
         <v>100</v>
       </c>
-      <c r="J12" s="12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <v>2</v>
-      </c>
-      <c r="L12" s="12">
-        <v>2</v>
-      </c>
-      <c r="M12" s="12">
-        <v>2</v>
-      </c>
-      <c r="N12" s="12">
-        <v>2</v>
-      </c>
-      <c r="O12" s="12">
-        <v>2</v>
-      </c>
-      <c r="P12" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="12">
-        <v>2</v>
-      </c>
-      <c r="R12" s="12">
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10">
+        <v>2</v>
+      </c>
+      <c r="L12" s="10">
+        <v>2</v>
+      </c>
+      <c r="M12" s="10">
+        <v>2</v>
+      </c>
+      <c r="N12" s="10">
+        <v>2</v>
+      </c>
+      <c r="O12" s="10">
+        <v>2</v>
+      </c>
+      <c r="P12" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>2</v>
+      </c>
+      <c r="R12" s="10">
         <v>2</v>
       </c>
       <c r="S12">
@@ -1802,58 +1792,58 @@
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+      <c r="A13" s="10">
         <v>5</v>
       </c>
-      <c r="B13" s="12">
-        <v>0</v>
-      </c>
-      <c r="C13" s="12">
-        <v>2</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0</v>
-      </c>
-      <c r="E13" s="12">
-        <v>0</v>
-      </c>
-      <c r="F13" s="13">
-        <v>2</v>
-      </c>
-      <c r="G13" s="12">
+      <c r="B13" s="10">
+        <v>2</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11">
+        <v>2</v>
+      </c>
+      <c r="F13" s="10">
         <v>610</v>
       </c>
-      <c r="H13" s="12">
-        <v>1</v>
-      </c>
-      <c r="I13" s="12">
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10">
         <v>100</v>
       </c>
-      <c r="J13" s="12">
-        <v>0</v>
-      </c>
-      <c r="K13" s="12">
-        <v>2</v>
-      </c>
-      <c r="L13" s="12">
-        <v>0</v>
-      </c>
-      <c r="M13" s="12">
-        <v>2</v>
-      </c>
-      <c r="N13" s="12">
-        <v>2</v>
-      </c>
-      <c r="O13" s="12">
-        <v>2</v>
-      </c>
-      <c r="P13" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q13" s="12">
-        <v>2</v>
-      </c>
-      <c r="R13" s="12">
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="11">
+        <v>0</v>
+      </c>
+      <c r="K13" s="10">
+        <v>2</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0</v>
+      </c>
+      <c r="M13" s="10">
+        <v>2</v>
+      </c>
+      <c r="N13" s="10">
+        <v>2</v>
+      </c>
+      <c r="O13" s="10">
+        <v>2</v>
+      </c>
+      <c r="P13" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>2</v>
+      </c>
+      <c r="R13" s="10">
         <v>2</v>
       </c>
       <c r="S13">
@@ -1870,58 +1860,58 @@
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+      <c r="A14" s="10">
         <v>5</v>
       </c>
-      <c r="B14" s="12">
-        <v>0</v>
-      </c>
-      <c r="C14" s="12">
-        <v>2</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0</v>
-      </c>
-      <c r="E14" s="12">
-        <v>0</v>
-      </c>
-      <c r="F14" s="13">
-        <v>2</v>
-      </c>
-      <c r="G14" s="12">
+      <c r="B14" s="10">
+        <v>2</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="11">
+        <v>2</v>
+      </c>
+      <c r="F14" s="10">
         <v>610</v>
       </c>
-      <c r="H14" s="12">
-        <v>1</v>
-      </c>
-      <c r="I14" s="12">
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" s="10">
         <v>100</v>
       </c>
-      <c r="J14" s="12">
-        <v>0</v>
-      </c>
-      <c r="K14" s="12">
-        <v>2</v>
-      </c>
-      <c r="L14" s="12">
-        <v>2</v>
-      </c>
-      <c r="M14" s="12">
-        <v>2</v>
-      </c>
-      <c r="N14" s="12">
-        <v>2</v>
-      </c>
-      <c r="O14" s="12">
-        <v>0</v>
-      </c>
-      <c r="P14" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="12">
-        <v>2</v>
-      </c>
-      <c r="R14" s="12">
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="11">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <v>2</v>
+      </c>
+      <c r="L14" s="10">
+        <v>2</v>
+      </c>
+      <c r="M14" s="10">
+        <v>2</v>
+      </c>
+      <c r="N14" s="10">
+        <v>2</v>
+      </c>
+      <c r="O14" s="10">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>2</v>
+      </c>
+      <c r="R14" s="10">
         <v>2</v>
       </c>
       <c r="S14">
@@ -1938,58 +1928,58 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
+      <c r="A15" s="12">
         <v>5</v>
       </c>
-      <c r="B15" s="14">
-        <v>0</v>
-      </c>
-      <c r="C15" s="12">
-        <v>2</v>
-      </c>
-      <c r="D15" s="12">
-        <v>0</v>
-      </c>
-      <c r="E15" s="12">
-        <v>0</v>
-      </c>
-      <c r="F15" s="15">
-        <v>2</v>
-      </c>
-      <c r="G15" s="12">
+      <c r="B15" s="10">
+        <v>2</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>2</v>
+      </c>
+      <c r="F15" s="10">
         <v>610</v>
       </c>
-      <c r="H15" s="12">
-        <v>1</v>
-      </c>
-      <c r="I15" s="12">
+      <c r="G15" s="10">
+        <v>1</v>
+      </c>
+      <c r="H15" s="10">
         <v>100</v>
       </c>
-      <c r="J15" s="12">
-        <v>0</v>
-      </c>
-      <c r="K15" s="12">
-        <v>0</v>
-      </c>
-      <c r="L15" s="12">
-        <v>2</v>
-      </c>
-      <c r="M15" s="16">
-        <v>2</v>
-      </c>
-      <c r="N15" s="16">
-        <v>2</v>
-      </c>
-      <c r="O15" s="16">
-        <v>2</v>
-      </c>
-      <c r="P15" s="16">
-        <v>2</v>
-      </c>
-      <c r="Q15" s="16">
-        <v>2</v>
-      </c>
-      <c r="R15" s="12">
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="J15" s="11">
+        <v>0</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0</v>
+      </c>
+      <c r="L15" s="10">
+        <v>2</v>
+      </c>
+      <c r="M15" s="14">
+        <v>2</v>
+      </c>
+      <c r="N15" s="14">
+        <v>2</v>
+      </c>
+      <c r="O15" s="14">
+        <v>2</v>
+      </c>
+      <c r="P15" s="14">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>2</v>
+      </c>
+      <c r="R15" s="10">
         <v>2</v>
       </c>
       <c r="S15">
@@ -2006,58 +1996,58 @@
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="12">
+      <c r="A16" s="10">
         <v>1800</v>
       </c>
-      <c r="B16" s="12">
-        <v>0</v>
-      </c>
-      <c r="C16" s="12">
-        <v>2</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0</v>
-      </c>
-      <c r="E16" s="12">
-        <v>0</v>
-      </c>
-      <c r="F16" s="13">
-        <v>2</v>
-      </c>
-      <c r="G16" s="12">
+      <c r="B16" s="10">
+        <v>2</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
+        <v>2</v>
+      </c>
+      <c r="F16" s="10">
         <v>610</v>
       </c>
-      <c r="H16" s="12">
-        <v>1</v>
-      </c>
-      <c r="I16" s="12">
+      <c r="G16" s="10">
+        <v>1</v>
+      </c>
+      <c r="H16" s="10">
         <v>100</v>
       </c>
-      <c r="J16" s="12">
-        <v>0</v>
-      </c>
-      <c r="K16" s="12">
-        <v>2</v>
-      </c>
-      <c r="L16" s="12">
-        <v>2</v>
-      </c>
-      <c r="M16" s="12">
-        <v>2</v>
-      </c>
-      <c r="N16" s="12">
-        <v>2</v>
-      </c>
-      <c r="O16" s="12">
-        <v>2</v>
-      </c>
-      <c r="P16" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="12">
-        <v>2</v>
-      </c>
-      <c r="R16" s="12">
+      <c r="I16" s="10">
+        <v>0</v>
+      </c>
+      <c r="J16" s="11">
+        <v>0</v>
+      </c>
+      <c r="K16" s="10">
+        <v>2</v>
+      </c>
+      <c r="L16" s="10">
+        <v>2</v>
+      </c>
+      <c r="M16" s="10">
+        <v>2</v>
+      </c>
+      <c r="N16" s="10">
+        <v>2</v>
+      </c>
+      <c r="O16" s="10">
+        <v>2</v>
+      </c>
+      <c r="P16" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>2</v>
+      </c>
+      <c r="R16" s="10">
         <v>2</v>
       </c>
       <c r="S16">
@@ -2072,6 +2062,9 @@
       <c r="V16">
         <v>2</v>
       </c>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J17" s="16"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K2:Q2 K12:Q15 K8:P8 K4:Q7">
@@ -2124,12 +2117,12 @@
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F16">
+  <conditionalFormatting sqref="E2:E16">
     <cfRule type="cellIs" dxfId="1" priority="12" operator="greaterThan">
       <formula>1.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C16">
+  <conditionalFormatting sqref="B2:B16">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="greaterThan">
       <formula>1.5</formula>
     </cfRule>

</xml_diff>

<commit_message>
Aggiornato il Config.xlsx e tutte le librerie
</commit_message>
<xml_diff>
--- a/Config/Config_test.xlsx
+++ b/Config/Config_test.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITLOAIT\Documents\GitHub\OrionLogger\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66ECED1C-4F3C-4D64-BE63-74E000AA9DCF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D82E73C-5194-4AD0-8DA7-97D1B9CDA7D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
     <sheet name="Comandi" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -136,13 +136,13 @@
     <t>Weiss</t>
   </si>
   <si>
-    <t>Automatico</t>
-  </si>
-  <si>
     <t>CC_set point H</t>
   </si>
   <si>
     <t>COL_PORTA</t>
+  </si>
+  <si>
+    <t>Manuale</t>
   </si>
 </sst>
 </file>
@@ -161,7 +161,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AML4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,12 +918,12 @@
         <v>5</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -999,7 +999,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>14</v>

</xml_diff>